<commit_message>
Handling non-string exception in excel file
</commit_message>
<xml_diff>
--- a/datafiles/how2.xlsx
+++ b/datafiles/how2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\workspace eclipse\POIApache\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4133277D-E6BD-4A36-879A-3568603E6088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159E72A9-4BA1-4EF5-BC3C-BE2D5ECBB734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -42,13 +42,7 @@
     <t>Maria</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
     <t>Anna</t>
-  </si>
-  <si>
-    <t>PollWhite</t>
   </si>
 </sst>
 </file>
@@ -407,7 +401,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,19 +429,19 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="3">
+        <v>8523635</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="1">
+        <v>80080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set to accept only string cells, main list modified to String
</commit_message>
<xml_diff>
--- a/datafiles/how2.xlsx
+++ b/datafiles/how2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\workspace eclipse\POIApache\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159E72A9-4BA1-4EF5-BC3C-BE2D5ECBB734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F5A23-E102-4B9C-B531-6593733CFB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Anna</t>
+  </si>
+  <si>
+    <t>WDPE059A64</t>
+  </si>
+  <si>
+    <t>WLPE058669A</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,8 +435,8 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
-        <v>8523635</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,8 +446,8 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
-        <v>80080</v>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>